<commit_message>
Add new Parse Examples
</commit_message>
<xml_diff>
--- a/CSV/pe.xlsx
+++ b/CSV/pe.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="237">
   <si>
     <t>Мебель</t>
   </si>
@@ -723,6 +723,12 @@
   </si>
   <si>
     <t>Authentication</t>
+  </si>
+  <si>
+    <t>Watermark</t>
+  </si>
+  <si>
+    <t>No price</t>
   </si>
 </sst>
 </file>
@@ -1452,8 +1458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C6:F148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1616,6 +1622,9 @@
       <c r="D22" s="5" t="s">
         <v>61</v>
       </c>
+      <c r="F22" s="1" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="23" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D23" s="5" t="s">
@@ -1692,88 +1701,127 @@
       <c r="D31" s="5" t="s">
         <v>75</v>
       </c>
+      <c r="F31" s="1" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="32" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D32" s="5" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F32" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="33" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D33" s="5" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F33" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="34" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D34" s="5" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F34" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="35" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D35" s="5" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="36" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="F35" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="36" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D36" s="5" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="37" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="F36" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="37" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D37" s="5" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F37" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="38" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D38" s="5" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F38" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="39" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D39" s="5" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="40" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="F39" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="40" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D40" s="5" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F40" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="41" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D41" s="5" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="42" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="F41" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="42" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D42" s="5" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="43" spans="4:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="F42" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="43" spans="4:6" ht="45" x14ac:dyDescent="0.25">
       <c r="D43" s="5" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F43" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="44" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D44" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D45" s="5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D46" s="5" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D47" s="5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D48" s="5" t="s">
         <v>92</v>
       </c>

</xml_diff>

<commit_message>
Found mistake in merging. File had not closed while pushing
</commit_message>
<xml_diff>
--- a/CSV/pe.xlsx
+++ b/CSV/pe.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="237">
   <si>
     <t>Мебель</t>
   </si>
@@ -1458,8 +1458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C6:F148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45:F132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1810,498 +1810,762 @@
       <c r="D45" s="5" t="s">
         <v>89</v>
       </c>
+      <c r="F45" s="1" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="46" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D46" s="5" t="s">
         <v>90</v>
       </c>
+      <c r="F46" s="1" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="47" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D47" s="5" t="s">
         <v>91</v>
       </c>
+      <c r="F47" s="1" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="48" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D48" s="5" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F48" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="49" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D49" s="5" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F49" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="50" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D50" s="5" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F50" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="51" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D51" s="5" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="52" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="F51" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="52" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D52" s="5" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F52" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="53" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D53" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F53" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="54" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D54" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F54" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="55" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D55" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F55" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="56" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D56" s="5" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F56" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="57" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D57" s="5" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="58" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="F57" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="58" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D58" s="5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F58" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="59" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D59" s="5" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F59" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="60" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D60" s="5" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F60" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="61" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D61" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F61" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="62" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D62" s="5" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F62" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="63" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D63" s="5" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F63" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="64" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D64" s="5" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F64" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="65" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D65" s="5" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F65" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="66" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D66" s="5" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="67" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="F66" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="67" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D67" s="5" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="68" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="F67" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="68" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D68" s="5" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="69" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="F68" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="69" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D69" s="5" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F69" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="70" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D70" s="5" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F70" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="71" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D71" s="5" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F71" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="72" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D72" s="5" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F72" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="73" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D73" s="5" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F73" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="74" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D74" s="5" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F74" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="75" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D75" s="5" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="76" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="F75" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="76" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D76" s="5" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F76" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="77" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D77" s="5" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F77" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="78" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D78" s="5" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F78" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="79" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D79" s="5" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F79" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="80" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D80" s="5" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F80" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="81" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D81" s="5" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F81" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="82" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D82" s="5" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F82" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="83" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D83" s="5" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="84" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="F83" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="84" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D84" s="5" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="85" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="F84" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="85" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D85" s="5" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F85" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="86" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D86" s="5" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F86" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="87" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D87" s="5" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="88" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="F87" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="88" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D88" s="5" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="89" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="F88" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="89" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D89" s="5" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="90" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="F89" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="90" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D90" s="5" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F90" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="91" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D91" s="5" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F91" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="92" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D92" s="5" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="93" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="F92" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="93" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D93" s="5" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="94" spans="4:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="F93" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="94" spans="4:6" ht="45" x14ac:dyDescent="0.25">
       <c r="D94" s="5" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="95" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="F94" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="95" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D95" s="5" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="96" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F95" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="96" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D96" s="5" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="97" spans="4:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="F96" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="97" spans="4:6" ht="45" x14ac:dyDescent="0.25">
       <c r="D97" s="5" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F97" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="98" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D98" s="5" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F98" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="99" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D99" s="5" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="100" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="F99" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="100" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D100" s="5" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F100" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="101" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D101" s="5" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="102" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="F101" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="102" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D102" s="5" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="103" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F102" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="103" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D103" s="5" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="104" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="F103" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="104" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D104" s="5" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="105" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F104" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="105" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D105" s="5" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="106" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F105" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="106" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D106" s="5" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="107" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F106" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="107" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D107" s="5" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="108" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F107" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="108" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D108" s="5" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="109" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F108" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="109" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D109" s="5" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="110" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="F109" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="110" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D110" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="111" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F110" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="111" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D111" s="5" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="112" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F111" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="112" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D112" s="5" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="113" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F112" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="113" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D113" s="5" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="114" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="F113" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="114" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D114" s="5" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="115" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="F114" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="115" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D115" s="5" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="116" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F115" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="116" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D116" s="5" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="117" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F116" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="117" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D117" s="5" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="118" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="F117" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="118" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D118" s="5" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="119" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="F118" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="119" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D119" s="5" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="120" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F119" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="120" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D120" s="5" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="121" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F120" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="121" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D121" s="5" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="122" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F121" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="122" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D122" s="5" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="123" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="F122" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="123" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D123" s="5" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="124" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F123" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="124" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D124" s="5" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="125" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F124" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="125" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D125" s="5" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="126" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="F125" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="126" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D126" s="5" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="127" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F126" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="127" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D127" s="5" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="128" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F127" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="128" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D128" s="5" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="129" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F128" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="129" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D129" s="5" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="130" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="F129" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="130" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D130" s="5" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="131" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="F130" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="131" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D131" s="5" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="132" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F131" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="132" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D132" s="5" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="133" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F132" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="133" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D133" s="5" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="134" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D134" s="5" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="135" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D135" s="5" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="136" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D136" s="5" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="137" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D137" s="5" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="138" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D138" s="5" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="139" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D139" s="5" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="140" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D140" s="5" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="141" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D141" s="5" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="142" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D142" s="5" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="143" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D143" s="5" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="144" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D144" s="5" t="s">
         <v>190</v>
       </c>

</xml_diff>

<commit_message>
Modified PE.xlsx file; Added archive VesnaKirov
</commit_message>
<xml_diff>
--- a/CSV/pe.xlsx
+++ b/CSV/pe.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="237">
   <si>
     <t>Мебель</t>
   </si>
@@ -1458,8 +1458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C6:F148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45:F132"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1629,6 +1629,9 @@
     <row r="23" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D23" s="5" t="s">
         <v>62</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="24" spans="4:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added new Parse Example: Playdorado
</commit_message>
<xml_diff>
--- a/CSV/pe.xlsx
+++ b/CSV/pe.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="237">
   <si>
     <t>Мебель</t>
   </si>
@@ -1458,8 +1458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C6:F148"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="D144" sqref="D144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2517,6 +2517,9 @@
       <c r="D133" s="5" t="s">
         <v>179</v>
       </c>
+      <c r="F133" s="1" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="134" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D134" s="5" t="s">
@@ -2573,22 +2576,25 @@
         <v>190</v>
       </c>
     </row>
-    <row r="145" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D145" s="5" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="146" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F145" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="146" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D146" s="5" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="147" spans="4:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="147" spans="4:6" ht="45" x14ac:dyDescent="0.25">
       <c r="D147" s="5" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="148" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D148" s="5" t="s">
         <v>223</v>
       </c>
@@ -2739,6 +2745,7 @@
     <hyperlink ref="D148" r:id="rId142"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId143"/>
 </worksheet>
 </file>
 

</xml_diff>